<commit_message>
temp fix for report for client
</commit_message>
<xml_diff>
--- a/Projects/MONDELEZUS/Data/KENGINE_MONDELEZUS_V1.xlsx
+++ b/Projects/MONDELEZUS/Data/KENGINE_MONDELEZUS_V1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -390,17 +390,17 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.6720647773279"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1295546558704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -506,14 +506,14 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="9" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="51.2024291497976"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="51.6315789473684"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="9" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="9" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="10" width="9.10526315789474"/>
@@ -560,13 +560,13 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
new template changes and code to reflect it.
</commit_message>
<xml_diff>
--- a/Projects/MONDELEZUS/Data/KENGINE_MONDELEZUS_V1.xlsx
+++ b/Projects/MONDELEZUS/Data/KENGINE_MONDELEZUS_V1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -45,25 +45,22 @@
     <t xml:space="preserve">Sweets</t>
   </si>
   <si>
-    <t xml:space="preserve">Candy/Chocolate Primary Location</t>
+    <t xml:space="preserve">Candy/Chocolate Primary Location,Candy/Chocolate Secondary Location</t>
   </si>
   <si>
     <t xml:space="preserve">Chewing Gum &amp; Mints</t>
   </si>
   <si>
-    <t xml:space="preserve">Chewing Gum Primary Location</t>
+    <t xml:space="preserve">Chewing Gum Primary Location ,Chewing Gum Secondary Location</t>
   </si>
   <si>
     <t xml:space="preserve">Chocolate</t>
   </si>
   <si>
-    <t xml:space="preserve">Candy/Chocolate Secondary Location</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cookies &amp; Crackers</t>
   </si>
   <si>
-    <t xml:space="preserve">Biscuits (Cookies &amp; Crackers) Primary Location</t>
+    <t xml:space="preserve">Biscuits (Cookies &amp; Crackers) Primary Location,Biscuits (Cookies &amp; Crackers) Secondary Location</t>
   </si>
   <si>
     <t xml:space="preserve">Cough</t>
@@ -391,16 +388,16 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1295546558704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -418,7 +415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -446,7 +443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -456,11 +453,11 @@
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -468,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,10 +479,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -507,13 +504,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="D4 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="9" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="52.5951417004049"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="9" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="9" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="10" width="9.10526315789474"/>
@@ -522,21 +519,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="70.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>20</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>1</v>
@@ -561,57 +558,57 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="D4 D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,13 +624,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
template update to match db change
</commit_message>
<xml_diff>
--- a/Projects/MONDELEZUS/Data/KENGINE_MONDELEZUS_V1.xlsx
+++ b/Projects/MONDELEZUS/Data/KENGINE_MONDELEZUS_V1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">Chewing Gum &amp; Mints</t>
   </si>
   <si>
-    <t xml:space="preserve">Chewing Gum Primary Location ,Chewing Gum Secondary Location</t>
+    <t xml:space="preserve">Chewing Gum Primary Location,Chewing Gum Secondary Location</t>
   </si>
   <si>
     <t xml:space="preserve">Chocolate</t>
@@ -388,16 +388,16 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.9878542510121"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -504,13 +504,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="D4 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="9" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="53.0242914979757"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="9" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="9" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="10" width="9.10526315789474"/>
@@ -558,12 +558,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="D4 D21"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>